<commit_message>
fix: ponteiros das primitivas em instancias em enderecos diferentes
</commit_message>
<xml_diff>
--- a/data/instancias/Instancia - Facil (Comp).xlsx
+++ b/data/instancias/Instancia - Facil (Comp).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="420">
   <si>
     <t>ID</t>
   </si>
@@ -1249,10 +1249,31 @@
     <t>Técnico</t>
   </si>
   <si>
-    <t>Técnico em Administração</t>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>Nome</t>
   </si>
   <si>
     <t xml:space="preserve">Periodo </t>
+  </si>
+  <si>
+    <t>Ciência da Computação - Primeiro Periodo</t>
+  </si>
+  <si>
+    <t>Ciência da Computação - Terceiro Periodo</t>
+  </si>
+  <si>
+    <t>Ciência da Computação - Quinto Periodo</t>
+  </si>
+  <si>
+    <t>Ciência da Computação - Setimo Periodo</t>
+  </si>
+  <si>
+    <t>Técnico em Informática - Terceiro Semestre</t>
+  </si>
+  <si>
+    <t>Técnico em Informática - Quarto Semestre</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1410,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1499,7 +1520,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="9" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1515,6 +1536,9 @@
     </xf>
     <xf borderId="4" fillId="9" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="9" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -28369,6 +28393,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="35" t="s">
@@ -28377,31 +28404,33 @@
       <c r="B1" s="36" t="s">
         <v>411</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>412</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="39"/>
       <c r="L1" s="39"/>
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
@@ -28416,6 +28445,7 @@
       <c r="W1" s="39"/>
       <c r="X1" s="39"/>
       <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
     </row>
     <row r="2">
       <c r="A2" s="40" t="s">
@@ -28424,38 +28454,40 @@
       <c r="B2" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="42" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="32" t="str">
+      <c r="E2" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A2)))"),"183494,182310,182309,182311,182312")</f>
         <v>183494,182310,182309,182311,182312</v>
       </c>
-      <c r="E2" s="33" t="str">
-        <f t="shared" ref="E2:E7" si="1">ifs(C2 = "Manhã", "7-16", C2 = "Tarde", "1-6,13-16", C2 = "Noite", "1-12", C2 = "Integral", "13-16")</f>
+      <c r="F2" s="33" t="str">
+        <f t="shared" ref="F2:F7" si="1">ifs(D2 = "Manhã", "7-16", D2 = "Tarde", "1-6,13-16", D2 = "Noite", "1-12", D2 = "Integral", "13-16")</f>
         <v>1-6,13-16</v>
       </c>
-      <c r="F2" s="33" t="str">
-        <f t="shared" ref="F2:F7" si="2">ifs(C2 = "Manhã", "7-16", C2 = "Tarde", "1-6,13-16", C2 = "Noite", "1-12", C2 = "Integral", "13-16")</f>
+      <c r="G2" s="33" t="str">
+        <f t="shared" ref="G2:G7" si="2">ifs(D2 = "Manhã", "7-16", D2 = "Tarde", "1-6,13-16", D2 = "Noite", "1-12", D2 = "Integral", "13-16")</f>
         <v>1-6,13-16</v>
       </c>
-      <c r="G2" s="33" t="str">
-        <f t="shared" ref="G2:G7" si="3">ifs(C2 = "Manhã", "7-16", C2 = "Tarde", "1-6,13-16", C2 = "Noite", "1-12", C2 = "Integral", "13-16")</f>
+      <c r="H2" s="33" t="str">
+        <f t="shared" ref="H2:H7" si="3">ifs(D2 = "Manhã", "7-16", D2 = "Tarde", "1-6,13-16", D2 = "Noite", "1-12", D2 = "Integral", "13-16")</f>
         <v>1-6,13-16</v>
       </c>
-      <c r="H2" s="33" t="str">
-        <f t="shared" ref="H2:H7" si="4">ifs(C2 = "Manhã", "7-16", C2 = "Tarde", "1-6,13-16", C2 = "Noite", "1-12", C2 = "Integral", "13-16")</f>
+      <c r="I2" s="33" t="str">
+        <f t="shared" ref="I2:I7" si="4">ifs(D2 = "Manhã", "7-16", D2 = "Tarde", "1-6,13-16", D2 = "Noite", "1-12", D2 = "Integral", "13-16")</f>
         <v>1-6,13-16</v>
       </c>
-      <c r="I2" s="33" t="str">
-        <f t="shared" ref="I2:I7" si="5">ifs(C2 = "Manhã", "7-16", C2 = "Tarde", "1-6,13-16", C2 = "Noite", "1-12", C2 = "Integral", "13-16")</f>
+      <c r="J2" s="33" t="str">
+        <f t="shared" ref="J2:J7" si="5">ifs(D2 = "Manhã", "7-16", D2 = "Tarde", "1-6,13-16", D2 = "Noite", "1-12", D2 = "Integral", "13-16")</f>
         <v>1-6,13-16</v>
       </c>
-      <c r="J2" s="33" t="str">
-        <f t="shared" ref="J2:J7" si="6">ifs(C2 = "Manhã", "1-16", C2 = "Tarde", "1-16", C2 = "Noite", "12-16", C2 = "Integral", "1-16")</f>
+      <c r="K2" s="33" t="str">
+        <f t="shared" ref="K2:K7" si="6">ifs(D2 = "Manhã", "1-16", D2 = "Tarde", "1-16", D2 = "Noite", "12-16", D2 = "Integral", "1-16")</f>
         <v>1-16</v>
       </c>
-      <c r="K2" s="39"/>
       <c r="L2" s="39"/>
       <c r="M2" s="39"/>
       <c r="N2" s="39"/>
@@ -28470,6 +28502,7 @@
       <c r="W2" s="39"/>
       <c r="X2" s="39"/>
       <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
@@ -28478,38 +28511,40 @@
       <c r="B3" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="32" t="str">
+      <c r="E3" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A3)))"),"182313,182314,182315,182316,182317,182318")</f>
         <v>182313,182314,182315,182316,182317,182318</v>
       </c>
-      <c r="E3" s="33" t="str">
+      <c r="F3" s="33" t="str">
         <f t="shared" si="1"/>
         <v>7-16</v>
       </c>
-      <c r="F3" s="33" t="str">
+      <c r="G3" s="33" t="str">
         <f t="shared" si="2"/>
         <v>7-16</v>
       </c>
-      <c r="G3" s="33" t="str">
+      <c r="H3" s="33" t="str">
         <f t="shared" si="3"/>
         <v>7-16</v>
       </c>
-      <c r="H3" s="33" t="str">
+      <c r="I3" s="33" t="str">
         <f t="shared" si="4"/>
         <v>7-16</v>
       </c>
-      <c r="I3" s="33" t="str">
+      <c r="J3" s="33" t="str">
         <f t="shared" si="5"/>
         <v>7-16</v>
       </c>
-      <c r="J3" s="33" t="str">
+      <c r="K3" s="33" t="str">
         <f t="shared" si="6"/>
         <v>1-16</v>
       </c>
-      <c r="K3" s="39"/>
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
       <c r="N3" s="39"/>
@@ -28524,6 +28559,7 @@
       <c r="W3" s="39"/>
       <c r="X3" s="39"/>
       <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
@@ -28532,38 +28568,40 @@
       <c r="B4" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="42" t="s">
+        <v>416</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="32" t="str">
+      <c r="E4" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A4)))"),"182319,182320,183866,182321,182322,182323")</f>
         <v>182319,182320,183866,182321,182322,182323</v>
       </c>
-      <c r="E4" s="33" t="str">
+      <c r="F4" s="33" t="str">
         <f t="shared" si="1"/>
         <v>1-6,13-16</v>
       </c>
-      <c r="F4" s="33" t="str">
+      <c r="G4" s="33" t="str">
         <f t="shared" si="2"/>
         <v>1-6,13-16</v>
       </c>
-      <c r="G4" s="33" t="str">
+      <c r="H4" s="33" t="str">
         <f t="shared" si="3"/>
         <v>1-6,13-16</v>
       </c>
-      <c r="H4" s="33" t="str">
+      <c r="I4" s="33" t="str">
         <f t="shared" si="4"/>
         <v>1-6,13-16</v>
       </c>
-      <c r="I4" s="33" t="str">
+      <c r="J4" s="33" t="str">
         <f t="shared" si="5"/>
         <v>1-6,13-16</v>
       </c>
-      <c r="J4" s="33" t="str">
+      <c r="K4" s="33" t="str">
         <f t="shared" si="6"/>
         <v>1-16</v>
       </c>
-      <c r="K4" s="39"/>
       <c r="L4" s="39"/>
       <c r="M4" s="39"/>
       <c r="N4" s="39"/>
@@ -28578,6 +28616,7 @@
       <c r="W4" s="39"/>
       <c r="X4" s="39"/>
       <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
@@ -28586,38 +28625,40 @@
       <c r="B5" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="32" t="str">
+      <c r="E5" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A5)))"),"182324,182325,183867,182326,182327")</f>
         <v>182324,182325,183867,182326,182327</v>
       </c>
-      <c r="E5" s="33" t="str">
+      <c r="F5" s="33" t="str">
         <f t="shared" si="1"/>
         <v>7-16</v>
       </c>
-      <c r="F5" s="33" t="str">
+      <c r="G5" s="33" t="str">
         <f t="shared" si="2"/>
         <v>7-16</v>
       </c>
-      <c r="G5" s="33" t="str">
+      <c r="H5" s="33" t="str">
         <f t="shared" si="3"/>
         <v>7-16</v>
       </c>
-      <c r="H5" s="33" t="str">
+      <c r="I5" s="33" t="str">
         <f t="shared" si="4"/>
         <v>7-16</v>
       </c>
-      <c r="I5" s="33" t="str">
+      <c r="J5" s="33" t="str">
         <f t="shared" si="5"/>
         <v>7-16</v>
       </c>
-      <c r="J5" s="33" t="str">
+      <c r="K5" s="33" t="str">
         <f t="shared" si="6"/>
         <v>1-16</v>
       </c>
-      <c r="K5" s="39"/>
       <c r="L5" s="39"/>
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
@@ -28632,6 +28673,7 @@
       <c r="W5" s="39"/>
       <c r="X5" s="39"/>
       <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
     </row>
     <row r="6">
       <c r="A6" s="40" t="s">
@@ -28640,38 +28682,40 @@
       <c r="B6" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="42" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="32" t="str">
+      <c r="E6" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A6)))"),"183895,183669,183667")</f>
         <v>183895,183669,183667</v>
       </c>
-      <c r="E6" s="33" t="str">
+      <c r="F6" s="33" t="str">
         <f t="shared" si="1"/>
         <v>1-12</v>
       </c>
-      <c r="F6" s="33" t="str">
+      <c r="G6" s="33" t="str">
         <f t="shared" si="2"/>
         <v>1-12</v>
       </c>
-      <c r="G6" s="33" t="str">
+      <c r="H6" s="33" t="str">
         <f t="shared" si="3"/>
         <v>1-12</v>
       </c>
-      <c r="H6" s="33" t="str">
+      <c r="I6" s="33" t="str">
         <f t="shared" si="4"/>
         <v>1-12</v>
       </c>
-      <c r="I6" s="33" t="str">
+      <c r="J6" s="33" t="str">
         <f t="shared" si="5"/>
         <v>1-12</v>
       </c>
-      <c r="J6" s="33" t="str">
+      <c r="K6" s="33" t="str">
         <f t="shared" si="6"/>
         <v>12-16</v>
       </c>
-      <c r="K6" s="39"/>
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
       <c r="N6" s="39"/>
@@ -28686,6 +28730,7 @@
       <c r="W6" s="39"/>
       <c r="X6" s="39"/>
       <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s">
@@ -28694,38 +28739,40 @@
       <c r="B7" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="32" t="str">
+      <c r="E7" s="32" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("JOIN("","",FILTER(Disciplinas!A:A, regexmatch(Disciplinas!E:E, A7)))"),"183670,183672,183673")</f>
         <v>183670,183672,183673</v>
       </c>
-      <c r="E7" s="33" t="str">
+      <c r="F7" s="33" t="str">
         <f t="shared" si="1"/>
         <v>1-12</v>
       </c>
-      <c r="F7" s="33" t="str">
+      <c r="G7" s="33" t="str">
         <f t="shared" si="2"/>
         <v>1-12</v>
       </c>
-      <c r="G7" s="33" t="str">
+      <c r="H7" s="33" t="str">
         <f t="shared" si="3"/>
         <v>1-12</v>
       </c>
-      <c r="H7" s="33" t="str">
+      <c r="I7" s="33" t="str">
         <f t="shared" si="4"/>
         <v>1-12</v>
       </c>
-      <c r="I7" s="33" t="str">
+      <c r="J7" s="33" t="str">
         <f t="shared" si="5"/>
         <v>1-12</v>
       </c>
-      <c r="J7" s="33" t="str">
+      <c r="K7" s="33" t="str">
         <f t="shared" si="6"/>
         <v>12-16</v>
       </c>
-      <c r="K7" s="39"/>
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
       <c r="N7" s="39"/>
@@ -28740,6 +28787,7 @@
       <c r="W7" s="39"/>
       <c r="X7" s="39"/>
       <c r="Y7" s="39"/>
+      <c r="Z7" s="39"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>